<commit_message>
feat: adding profile setting
</commit_message>
<xml_diff>
--- a/public/templates/mahasiswa_template.xlsx
+++ b/public/templates/mahasiswa_template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Laravel\kampus-merdeka-ung\public\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moham\OneDrive\Desktop\kampus-merdeka-ung\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD498FD6-E846-43D2-8372-61509B805F44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84A9FC94-1108-4EE6-8D69-3841AF099B29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,21 +25,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>NAMA</t>
   </si>
   <si>
-    <t>PROVINSI</t>
+    <t>NIM</t>
   </si>
   <si>
-    <t>KABUPATEN</t>
+    <t>KODE_PROGRAM_STUDI</t>
   </si>
   <si>
-    <t>KECAMATAN</t>
-  </si>
-  <si>
-    <t>KELURAHAN</t>
+    <t>ANGKATAN</t>
   </si>
 </sst>
 </file>
@@ -364,7 +361,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
@@ -377,12 +374,12 @@
     <col min="5" max="5" width="34.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
@@ -390,9 +387,6 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>